<commit_message>
unsorted excel validation and json validator skip
</commit_message>
<xml_diff>
--- a/UnitTestUTDataValidator/excel/sample-tipe-data.xlsx
+++ b/UnitTestUTDataValidator/excel/sample-tipe-data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurizalandika/RiderProjects/ut_data_validator/UnitTestUTDataValidator/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4EE7FB-42F8-1E40-846A-D8B080C12D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CA872D-883D-FE41-BE26-C52CF04678A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{3BF7958D-2346-C140-9764-D7771D091A66}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
     <sheet name="expected" sheetId="2" r:id="rId2"/>
+    <sheet name="unsorted" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>table: SampleTable</t>
   </si>
@@ -530,7 +531,125 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A1:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44562</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44563</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4" s="4">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44564</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4">
+        <v>20.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D429E-4AA8-1241-90D1-2DE9FCE8C090}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,48 +708,48 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>44563</v>
+        <v>44564</v>
       </c>
       <c r="D4" s="2">
-        <v>6.9444444444444447E-4</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4">
-        <v>20.2</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>44564</v>
+        <v>44563</v>
       </c>
       <c r="D5" s="2">
-        <v>1.3888888888888889E-3</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="4">
-        <v>20.3</v>
+        <v>20.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>